<commit_message>
completed assgm1 and updated assgnm2 questions
</commit_message>
<xml_diff>
--- a/excel_automations/AmazonBooks.xlsx
+++ b/excel_automations/AmazonBooks.xlsx
@@ -8,14 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\training_Sarah\excel_automations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41AAA9A8-5973-45A3-A3C6-A04FFCF51A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7772F98-F7CB-49DA-8AFE-EE1C9799C1B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$603</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2321,13 +2335,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+  <sheetPr filterMode="1">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:G603"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2365,9 +2379,7 @@
       <c r="C2" s="2">
         <v>4.7</v>
       </c>
-      <c r="D2" s="2">
-        <v>17350</v>
-      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="2">
         <v>8</v>
       </c>
@@ -2378,7 +2390,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -2424,7 +2436,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -2470,7 +2482,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -2493,7 +2505,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -2516,7 +2528,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -2562,7 +2574,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>26</v>
       </c>
@@ -2585,7 +2597,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -2608,7 +2620,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>673</v>
       </c>
@@ -2675,7 +2687,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>32</v>
       </c>
@@ -2836,7 +2848,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>45</v>
       </c>
@@ -2859,7 +2871,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>45</v>
       </c>
@@ -2882,7 +2894,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>47</v>
       </c>
@@ -2905,7 +2917,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>675</v>
       </c>
@@ -2949,7 +2961,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>51</v>
       </c>
@@ -3271,7 +3283,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>74</v>
       </c>
@@ -3317,7 +3329,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>77</v>
       </c>
@@ -3340,7 +3352,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>77</v>
       </c>
@@ -3363,7 +3375,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>79</v>
       </c>
@@ -3455,7 +3467,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>87</v>
       </c>
@@ -3478,7 +3490,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>87</v>
       </c>
@@ -3501,7 +3513,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>87</v>
       </c>
@@ -3616,7 +3628,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>93</v>
       </c>
@@ -3685,7 +3697,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>98</v>
       </c>
@@ -3708,7 +3720,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>98</v>
       </c>
@@ -3777,7 +3789,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>104</v>
       </c>
@@ -3800,7 +3812,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>106</v>
       </c>
@@ -3823,7 +3835,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>107</v>
       </c>
@@ -3846,7 +3858,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>108</v>
       </c>
@@ -3869,7 +3881,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>108</v>
       </c>
@@ -3892,7 +3904,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>108</v>
       </c>
@@ -3915,7 +3927,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>108</v>
       </c>
@@ -4030,7 +4042,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>116</v>
       </c>
@@ -4053,7 +4065,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>117</v>
       </c>
@@ -4076,7 +4088,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>118</v>
       </c>
@@ -4122,7 +4134,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>121</v>
       </c>
@@ -4145,7 +4157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>121</v>
       </c>
@@ -4168,7 +4180,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>122</v>
       </c>
@@ -4214,7 +4226,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>125</v>
       </c>
@@ -4237,7 +4249,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>126</v>
       </c>
@@ -4260,7 +4272,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>127</v>
       </c>
@@ -4283,7 +4295,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>129</v>
       </c>
@@ -4306,7 +4318,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>130</v>
       </c>
@@ -4329,7 +4341,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>130</v>
       </c>
@@ -4352,7 +4364,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>131</v>
       </c>
@@ -4375,7 +4387,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>132</v>
       </c>
@@ -4398,7 +4410,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>133</v>
       </c>
@@ -4421,7 +4433,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>134</v>
       </c>
@@ -4582,7 +4594,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>144</v>
       </c>
@@ -4605,7 +4617,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>145</v>
       </c>
@@ -4697,7 +4709,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>150</v>
       </c>
@@ -4720,7 +4732,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>150</v>
       </c>
@@ -4743,7 +4755,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>152</v>
       </c>
@@ -4789,7 +4801,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>156</v>
       </c>
@@ -4812,7 +4824,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>158</v>
       </c>
@@ -4835,7 +4847,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>159</v>
       </c>
@@ -4858,7 +4870,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>159</v>
       </c>
@@ -4881,7 +4893,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>160</v>
       </c>
@@ -5065,7 +5077,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>167</v>
       </c>
@@ -5111,7 +5123,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>171</v>
       </c>
@@ -5134,7 +5146,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>171</v>
       </c>
@@ -5157,7 +5169,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>171</v>
       </c>
@@ -5226,7 +5238,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>177</v>
       </c>
@@ -5249,7 +5261,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>177</v>
       </c>
@@ -5272,7 +5284,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>177</v>
       </c>
@@ -5295,7 +5307,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>177</v>
       </c>
@@ -5318,7 +5330,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>177</v>
       </c>
@@ -5433,7 +5445,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>183</v>
       </c>
@@ -5456,7 +5468,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>185</v>
       </c>
@@ -5502,7 +5514,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>189</v>
       </c>
@@ -5525,7 +5537,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>189</v>
       </c>
@@ -5548,7 +5560,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>189</v>
       </c>
@@ -5686,7 +5698,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>195</v>
       </c>
@@ -5709,7 +5721,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>195</v>
       </c>
@@ -5732,7 +5744,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>195</v>
       </c>
@@ -5755,7 +5767,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>197</v>
       </c>
@@ -5778,7 +5790,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>197</v>
       </c>
@@ -5824,7 +5836,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" s="1" t="s">
         <v>201</v>
       </c>
@@ -5916,7 +5928,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="157" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" s="1" t="s">
         <v>208</v>
       </c>
@@ -5939,7 +5951,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="158" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" s="1" t="s">
         <v>209</v>
       </c>
@@ -5962,7 +5974,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" s="1" t="s">
         <v>210</v>
       </c>
@@ -5985,7 +5997,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" s="1" t="s">
         <v>212</v>
       </c>
@@ -6008,7 +6020,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" s="1" t="s">
         <v>213</v>
       </c>
@@ -6054,7 +6066,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" s="1" t="s">
         <v>216</v>
       </c>
@@ -6468,7 +6480,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="181" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
         <v>236</v>
       </c>
@@ -6491,7 +6503,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="182" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
         <v>238</v>
       </c>
@@ -6514,7 +6526,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="183" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
         <v>238</v>
       </c>
@@ -6537,7 +6549,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="184" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>240</v>
       </c>
@@ -6583,7 +6595,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="186" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>244</v>
       </c>
@@ -6606,7 +6618,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="187" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
         <v>246</v>
       </c>
@@ -6836,7 +6848,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="197" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
         <v>254</v>
       </c>
@@ -6859,7 +6871,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="198" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
         <v>255</v>
       </c>
@@ -7158,7 +7170,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="211" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
         <v>269</v>
       </c>
@@ -7411,7 +7423,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="222" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
         <v>282</v>
       </c>
@@ -7434,7 +7446,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="223" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" s="1" t="s">
         <v>284</v>
       </c>
@@ -7457,7 +7469,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="224" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
         <v>286</v>
       </c>
@@ -7480,7 +7492,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="225" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
         <v>288</v>
       </c>
@@ -7526,7 +7538,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="227" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
         <v>292</v>
       </c>
@@ -7549,7 +7561,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="228" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228" s="1" t="s">
         <v>292</v>
       </c>
@@ -7825,7 +7837,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="240" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A240" s="1" t="s">
         <v>306</v>
       </c>
@@ -7848,7 +7860,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="241" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A241" s="1" t="s">
         <v>306</v>
       </c>
@@ -7871,7 +7883,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="242" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242" s="1" t="s">
         <v>306</v>
       </c>
@@ -7940,7 +7952,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="245" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A245" s="1" t="s">
         <v>311</v>
       </c>
@@ -8032,7 +8044,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="249" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A249" s="1" t="s">
         <v>318</v>
       </c>
@@ -8055,7 +8067,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="250" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A250" s="1" t="s">
         <v>318</v>
       </c>
@@ -8078,7 +8090,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="251" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A251" s="1" t="s">
         <v>318</v>
       </c>
@@ -8101,7 +8113,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="252" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A252" s="1" t="s">
         <v>318</v>
       </c>
@@ -8124,7 +8136,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="253" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A253" s="1" t="s">
         <v>318</v>
       </c>
@@ -8147,7 +8159,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="254" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A254" s="1" t="s">
         <v>318</v>
       </c>
@@ -8170,7 +8182,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="255" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A255" s="1" t="s">
         <v>318</v>
       </c>
@@ -8193,7 +8205,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="256" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256" s="1" t="s">
         <v>318</v>
       </c>
@@ -8216,7 +8228,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="257" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A257" s="1" t="s">
         <v>320</v>
       </c>
@@ -8239,7 +8251,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="258" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A258" s="1" t="s">
         <v>321</v>
       </c>
@@ -8331,7 +8343,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="262" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A262" s="1" t="s">
         <v>326</v>
       </c>
@@ -8354,7 +8366,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="263" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A263" s="1" t="s">
         <v>327</v>
       </c>
@@ -8469,7 +8481,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="268" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A268" s="1" t="s">
         <v>332</v>
       </c>
@@ -8492,7 +8504,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="269" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A269" s="1" t="s">
         <v>334</v>
       </c>
@@ -8515,7 +8527,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="270" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A270" s="1" t="s">
         <v>334</v>
       </c>
@@ -8538,7 +8550,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="271" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A271" s="1" t="s">
         <v>334</v>
       </c>
@@ -8561,7 +8573,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="272" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A272" s="1" t="s">
         <v>336</v>
       </c>
@@ -8860,7 +8872,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="285" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A285" s="1" t="s">
         <v>341</v>
       </c>
@@ -8975,7 +8987,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="290" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A290" s="1" t="s">
         <v>347</v>
       </c>
@@ -8998,7 +9010,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="291" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A291" s="1" t="s">
         <v>347</v>
       </c>
@@ -9021,7 +9033,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="292" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A292" s="1" t="s">
         <v>349</v>
       </c>
@@ -9044,7 +9056,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="293" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A293" s="1" t="s">
         <v>351</v>
       </c>
@@ -9113,7 +9125,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="296" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A296" s="1" t="s">
         <v>354</v>
       </c>
@@ -9274,7 +9286,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="303" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A303" s="1" t="s">
         <v>365</v>
       </c>
@@ -9366,7 +9378,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="307" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A307" s="1" t="s">
         <v>368</v>
       </c>
@@ -9642,7 +9654,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="319" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A319" s="1" t="s">
         <v>376</v>
       </c>
@@ -10171,7 +10183,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="342" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A342" s="1" t="s">
         <v>391</v>
       </c>
@@ -10217,7 +10229,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="344" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A344" s="1" t="s">
         <v>395</v>
       </c>
@@ -10240,7 +10252,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="345" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A345" s="1" t="s">
         <v>395</v>
       </c>
@@ -10286,7 +10298,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="347" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A347" s="1" t="s">
         <v>399</v>
       </c>
@@ -10378,7 +10390,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="351" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A351" s="1" t="s">
         <v>406</v>
       </c>
@@ -10401,7 +10413,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="352" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A352" s="1" t="s">
         <v>406</v>
       </c>
@@ -10424,7 +10436,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="353" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A353" s="1" t="s">
         <v>408</v>
       </c>
@@ -10447,7 +10459,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="354" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A354" s="1" t="s">
         <v>408</v>
       </c>
@@ -10516,7 +10528,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="357" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A357" s="1" t="s">
         <v>412</v>
       </c>
@@ -10608,7 +10620,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="361" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A361" s="1" t="s">
         <v>417</v>
       </c>
@@ -10677,7 +10689,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="364" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A364" s="1" t="s">
         <v>422</v>
       </c>
@@ -10700,7 +10712,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="365" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A365" s="1" t="s">
         <v>422</v>
       </c>
@@ -10723,7 +10735,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="366" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A366" s="1" t="s">
         <v>422</v>
       </c>
@@ -10769,7 +10781,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="368" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A368" s="1" t="s">
         <v>426</v>
       </c>
@@ -10792,7 +10804,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="369" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A369" s="1" t="s">
         <v>428</v>
       </c>
@@ -10815,7 +10827,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="370" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A370" s="1" t="s">
         <v>428</v>
       </c>
@@ -10838,7 +10850,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="371" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A371" s="1" t="s">
         <v>428</v>
       </c>
@@ -10861,7 +10873,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="372" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A372" s="1" t="s">
         <v>428</v>
       </c>
@@ -11160,7 +11172,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="385" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A385" s="1" t="s">
         <v>434</v>
       </c>
@@ -11183,7 +11195,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="386" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A386" s="1" t="s">
         <v>435</v>
       </c>
@@ -11206,7 +11218,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="387" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A387" s="1" t="s">
         <v>435</v>
       </c>
@@ -11229,7 +11241,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="388" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A388" s="1" t="s">
         <v>437</v>
       </c>
@@ -11252,7 +11264,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="389" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A389" s="1" t="s">
         <v>437</v>
       </c>
@@ -11275,7 +11287,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="390" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A390" s="1" t="s">
         <v>439</v>
       </c>
@@ -11298,7 +11310,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="391" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A391" s="1" t="s">
         <v>440</v>
       </c>
@@ -11321,7 +11333,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="392" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A392" s="1" t="s">
         <v>441</v>
       </c>
@@ -11344,7 +11356,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="393" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A393" s="1" t="s">
         <v>441</v>
       </c>
@@ -11367,7 +11379,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="394" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A394" s="1" t="s">
         <v>442</v>
       </c>
@@ -11390,7 +11402,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="395" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A395" s="1" t="s">
         <v>442</v>
       </c>
@@ -11413,7 +11425,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="396" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A396" s="1" t="s">
         <v>444</v>
       </c>
@@ -11436,7 +11448,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="397" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A397" s="1" t="s">
         <v>444</v>
       </c>
@@ -11459,7 +11471,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="398" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A398" s="1" t="s">
         <v>446</v>
       </c>
@@ -11482,7 +11494,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="399" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A399" s="1" t="s">
         <v>446</v>
       </c>
@@ -11505,7 +11517,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="400" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A400" s="1" t="s">
         <v>446</v>
       </c>
@@ -11528,7 +11540,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="401" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A401" s="1" t="s">
         <v>448</v>
       </c>
@@ -11551,7 +11563,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="402" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A402" s="1" t="s">
         <v>449</v>
       </c>
@@ -11574,7 +11586,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="403" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A403" s="1" t="s">
         <v>451</v>
       </c>
@@ -11597,7 +11609,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="404" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A404" s="1" t="s">
         <v>453</v>
       </c>
@@ -11620,7 +11632,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="405" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A405" s="1" t="s">
         <v>455</v>
       </c>
@@ -11643,7 +11655,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="406" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A406" s="1" t="s">
         <v>457</v>
       </c>
@@ -11666,7 +11678,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="407" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A407" s="1" t="s">
         <v>457</v>
       </c>
@@ -11689,7 +11701,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="408" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A408" s="1" t="s">
         <v>457</v>
       </c>
@@ -11712,7 +11724,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="409" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A409" s="1" t="s">
         <v>457</v>
       </c>
@@ -11735,7 +11747,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="410" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A410" s="1" t="s">
         <v>459</v>
       </c>
@@ -11758,7 +11770,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="411" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A411" s="1" t="s">
         <v>460</v>
       </c>
@@ -11781,7 +11793,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="412" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A412" s="1" t="s">
         <v>461</v>
       </c>
@@ -11804,7 +11816,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="413" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A413" s="1" t="s">
         <v>461</v>
       </c>
@@ -11827,7 +11839,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="414" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A414" s="1" t="s">
         <v>462</v>
       </c>
@@ -11850,7 +11862,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="415" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A415" s="1" t="s">
         <v>462</v>
       </c>
@@ -12011,7 +12023,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="422" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A422" s="1" t="s">
         <v>469</v>
       </c>
@@ -12034,7 +12046,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="423" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A423" s="1" t="s">
         <v>469</v>
       </c>
@@ -12057,7 +12069,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="424" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A424" s="1" t="s">
         <v>470</v>
       </c>
@@ -12218,7 +12230,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="431" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A431" s="1" t="s">
         <v>476</v>
       </c>
@@ -12241,7 +12253,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="432" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A432" s="1" t="s">
         <v>477</v>
       </c>
@@ -12264,7 +12276,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="433" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A433" s="1" t="s">
         <v>478</v>
       </c>
@@ -12333,7 +12345,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="436" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A436" s="1" t="s">
         <v>483</v>
       </c>
@@ -12356,7 +12368,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="437" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A437" s="1" t="s">
         <v>484</v>
       </c>
@@ -12379,7 +12391,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="438" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A438" s="1" t="s">
         <v>486</v>
       </c>
@@ -12402,7 +12414,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="439" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A439" s="1" t="s">
         <v>488</v>
       </c>
@@ -12448,7 +12460,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="441" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A441" s="1" t="s">
         <v>491</v>
       </c>
@@ -12471,7 +12483,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="442" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A442" s="1" t="s">
         <v>491</v>
       </c>
@@ -12632,7 +12644,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="449" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A449" s="1" t="s">
         <v>496</v>
       </c>
@@ -12770,7 +12782,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="455" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A455" s="1" t="s">
         <v>505</v>
       </c>
@@ -12793,7 +12805,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="456" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A456" s="1" t="s">
         <v>505</v>
       </c>
@@ -12839,7 +12851,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="458" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A458" s="1" t="s">
         <v>509</v>
       </c>
@@ -12862,7 +12874,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="459" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A459" s="1" t="s">
         <v>510</v>
       </c>
@@ -12885,7 +12897,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="460" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A460" s="1" t="s">
         <v>511</v>
       </c>
@@ -12931,7 +12943,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="462" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A462" s="1" t="s">
         <v>514</v>
       </c>
@@ -12954,7 +12966,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="463" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A463" s="1" t="s">
         <v>515</v>
       </c>
@@ -12977,7 +12989,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="464" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A464" s="1" t="s">
         <v>515</v>
       </c>
@@ -13000,7 +13012,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="465" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A465" s="1" t="s">
         <v>517</v>
       </c>
@@ -13023,7 +13035,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="466" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A466" s="1" t="s">
         <v>518</v>
       </c>
@@ -13046,7 +13058,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="467" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A467" s="1" t="s">
         <v>520</v>
       </c>
@@ -13161,7 +13173,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="472" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A472" s="1" t="s">
         <v>524</v>
       </c>
@@ -13184,7 +13196,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="473" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A473" s="1" t="s">
         <v>525</v>
       </c>
@@ -13207,7 +13219,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="474" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A474" s="1" t="s">
         <v>526</v>
       </c>
@@ -13276,7 +13288,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="477" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A477" s="1" t="s">
         <v>531</v>
       </c>
@@ -13299,7 +13311,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="478" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A478" s="1" t="s">
         <v>532</v>
       </c>
@@ -13345,7 +13357,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="480" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A480" s="1" t="s">
         <v>535</v>
       </c>
@@ -13368,7 +13380,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="481" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A481" s="1" t="s">
         <v>535</v>
       </c>
@@ -13391,7 +13403,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="482" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A482" s="1" t="s">
         <v>535</v>
       </c>
@@ -13414,7 +13426,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="483" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A483" s="1" t="s">
         <v>535</v>
       </c>
@@ -13437,7 +13449,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="484" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A484" s="1" t="s">
         <v>535</v>
       </c>
@@ -13460,7 +13472,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="485" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A485" s="1" t="s">
         <v>535</v>
       </c>
@@ -13483,7 +13495,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="486" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A486" s="1" t="s">
         <v>535</v>
       </c>
@@ -13575,7 +13587,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="490" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="490" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A490" s="1" t="s">
         <v>539</v>
       </c>
@@ -13598,7 +13610,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="491" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="491" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A491" s="1" t="s">
         <v>539</v>
       </c>
@@ -13621,7 +13633,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="492" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A492" s="1" t="s">
         <v>539</v>
       </c>
@@ -13644,7 +13656,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="493" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="493" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A493" s="1" t="s">
         <v>539</v>
       </c>
@@ -13667,7 +13679,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="494" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="494" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A494" s="1" t="s">
         <v>541</v>
       </c>
@@ -13690,7 +13702,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="495" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="495" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A495" s="1" t="s">
         <v>541</v>
       </c>
@@ -13805,7 +13817,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="500" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="500" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A500" s="1" t="s">
         <v>549</v>
       </c>
@@ -14012,7 +14024,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="509" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="509" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A509" s="1" t="s">
         <v>559</v>
       </c>
@@ -14035,7 +14047,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="510" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="510" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A510" s="1" t="s">
         <v>559</v>
       </c>
@@ -14058,7 +14070,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="511" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="511" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A511" s="1" t="s">
         <v>559</v>
       </c>
@@ -14081,7 +14093,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="512" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="512" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A512" s="1" t="s">
         <v>559</v>
       </c>
@@ -14104,7 +14116,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="513" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="513" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A513" s="1" t="s">
         <v>559</v>
       </c>
@@ -14150,7 +14162,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="515" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="515" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A515" s="1" t="s">
         <v>561</v>
       </c>
@@ -14196,7 +14208,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="517" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="517" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A517" s="1" t="s">
         <v>565</v>
       </c>
@@ -14219,7 +14231,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="518" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="518" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A518" s="1" t="s">
         <v>566</v>
       </c>
@@ -14357,7 +14369,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="524" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="524" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A524" s="1" t="s">
         <v>569</v>
       </c>
@@ -14449,7 +14461,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="528" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="528" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A528" s="1" t="s">
         <v>574</v>
       </c>
@@ -14472,7 +14484,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="529" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="529" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A529" s="1" t="s">
         <v>576</v>
       </c>
@@ -14541,7 +14553,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="532" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="532" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A532" s="1" t="s">
         <v>582</v>
       </c>
@@ -14564,7 +14576,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="533" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="533" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A533" s="1" t="s">
         <v>583</v>
       </c>
@@ -14679,7 +14691,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="538" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="538" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A538" s="1" t="s">
         <v>591</v>
       </c>
@@ -14702,7 +14714,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="539" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="539" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A539" s="1" t="s">
         <v>593</v>
       </c>
@@ -14771,7 +14783,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="542" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="542" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A542" s="1" t="s">
         <v>599</v>
       </c>
@@ -14817,7 +14829,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="544" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="544" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A544" s="1" t="s">
         <v>603</v>
       </c>
@@ -14840,7 +14852,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="545" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="545" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A545" s="1" t="s">
         <v>603</v>
       </c>
@@ -14863,7 +14875,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="546" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="546" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A546" s="1" t="s">
         <v>603</v>
       </c>
@@ -14886,7 +14898,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="547" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="547" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A547" s="1" t="s">
         <v>603</v>
       </c>
@@ -14909,7 +14921,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="548" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="548" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A548" s="1" t="s">
         <v>603</v>
       </c>
@@ -14932,7 +14944,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="549" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="549" spans="1:7" ht="14.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A549" s="1" t="s">
         <v>605</v>
       </c>
@@ -15093,7 +15105,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="556" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="556" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A556" s="3" t="s">
         <v>591</v>
       </c>
@@ -15139,7 +15151,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="558" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="558" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A558" s="3" t="s">
         <v>614</v>
       </c>
@@ -15185,7 +15197,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="560" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="560" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A560" s="3" t="s">
         <v>238</v>
       </c>
@@ -15254,7 +15266,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="563" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="563" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A563" s="3" t="s">
         <v>357</v>
       </c>
@@ -15277,7 +15289,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="564" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="564" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A564" s="3" t="s">
         <v>621</v>
       </c>
@@ -15300,7 +15312,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="565" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="565" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A565" s="3" t="s">
         <v>622</v>
       </c>
@@ -15507,7 +15519,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="574" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="574" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A574" s="3" t="s">
         <v>633</v>
       </c>
@@ -15553,7 +15565,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="576" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="576" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A576" s="3" t="s">
         <v>286</v>
       </c>
@@ -15576,7 +15588,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="577" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="577" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A577" s="3" t="s">
         <v>637</v>
       </c>
@@ -15622,7 +15634,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="579" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="579" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A579" s="3" t="s">
         <v>640</v>
       </c>
@@ -15645,7 +15657,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="580" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="580" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A580" s="3" t="s">
         <v>642</v>
       </c>
@@ -15691,7 +15703,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="582" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="582" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A582" s="3" t="s">
         <v>646</v>
       </c>
@@ -15714,7 +15726,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="583" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="583" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A583" s="3" t="s">
         <v>177</v>
       </c>
@@ -15737,7 +15749,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="584" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="584" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A584" s="3" t="s">
         <v>77</v>
       </c>
@@ -15806,7 +15818,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="587" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="587" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A587" s="3" t="s">
         <v>649</v>
       </c>
@@ -15875,7 +15887,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="590" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="590" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A590" s="3" t="s">
         <v>541</v>
       </c>
@@ -15921,7 +15933,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="592" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="592" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A592" s="3" t="s">
         <v>654</v>
       </c>
@@ -15944,7 +15956,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="593" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="593" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A593" s="3" t="s">
         <v>656</v>
       </c>
@@ -15967,7 +15979,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="594" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="594" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A594" s="3" t="s">
         <v>657</v>
       </c>
@@ -15990,7 +16002,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="595" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="595" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A595" s="3" t="s">
         <v>658</v>
       </c>
@@ -16013,7 +16025,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="596" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="596" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A596" s="3" t="s">
         <v>660</v>
       </c>
@@ -16036,7 +16048,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="597" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="597" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A597" s="3" t="s">
         <v>661</v>
       </c>
@@ -16059,7 +16071,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="598" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="598" spans="1:7" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A598" s="3" t="s">
         <v>663</v>
       </c>
@@ -16198,6 +16210,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G603" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="Non Fiction"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>